<commit_message>
Reviewed Kojak & KojakPercolator (fixes #2)
Bundled Kojak and KojakPerc functions in a single KojakFunctions file (improves maintenance)
Fixed errors with calculating modpos in Kojak
Added functionality for long file names
</commit_message>
<xml_diff>
--- a/xTable_definition.xlsx
+++ b/xTable_definition.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>rawfile</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>np.nan</t>
+  </si>
+  <si>
+    <t>Missing data</t>
   </si>
 </sst>
 </file>
@@ -468,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +650,65 @@
         <v>28</v>
       </c>
     </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W4" t="s">
+        <v>35</v>
+      </c>
+      <c r="X4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed bug in xTable handling when "Merge files" is called
</commit_message>
<xml_diff>
--- a/xTable_definition.xlsx
+++ b/xTable_definition.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>rawfile</t>
   </si>
@@ -47,9 +47,6 @@
     <t>xlink2</t>
   </si>
   <si>
-    <t>xtype</t>
-  </si>
-  <si>
     <t>modmass1</t>
   </si>
   <si>
@@ -135,6 +132,72 @@
   </si>
   <si>
     <t>Missing data</t>
+  </si>
+  <si>
+    <t>charge of the precursor ion</t>
+  </si>
+  <si>
+    <t>Sequence of the longer (alpha) peptide</t>
+  </si>
+  <si>
+    <t>Sequence of the shorter (beta) peptide</t>
+  </si>
+  <si>
+    <t>Position of the cross-linker within the longer peptide</t>
+  </si>
+  <si>
+    <t>Position of the cross-linker within the shorter peptide</t>
+  </si>
+  <si>
+    <t>relative position of a modification within peptide 1 (;-delimited if multiple)</t>
+  </si>
+  <si>
+    <t>relative position of a modification within peptide 2 (;-delimited if multiple)</t>
+  </si>
+  <si>
+    <t>name of the modification(s) of peptide 1 (;-delimited if multiple)</t>
+  </si>
+  <si>
+    <t>name of the modification(s) of peptide 2 (;-delimited if multiple)</t>
+  </si>
+  <si>
+    <t>fasta-header of the protein corresponding to peptide 2</t>
+  </si>
+  <si>
+    <t>fasta-header of the protein corresponding to  peptide 1</t>
+  </si>
+  <si>
+    <t>Absolute position of the cross-linker in protein 1</t>
+  </si>
+  <si>
+    <t>Absolute position of the cross-linker in protein 2</t>
+  </si>
+  <si>
+    <t>inter, intra, homomultimeric, loop or mono</t>
+  </si>
+  <si>
+    <t>Absolute position of the first AA of peptide 1</t>
+  </si>
+  <si>
+    <t>Absolute position of the first AA of peptide 2</t>
+  </si>
+  <si>
+    <t>Identifier for the position of a cross-link between two proteins</t>
+  </si>
+  <si>
+    <t>not normalised score - cannot be used for comparison</t>
+  </si>
+  <si>
+    <t>If decoy or not</t>
+  </si>
+  <si>
+    <t>Which search engine was used</t>
+  </si>
+  <si>
+    <t>Scan number for the cross-link identification spectrum</t>
+  </si>
+  <si>
+    <t>Name of the corresponding rawfile</t>
   </si>
 </sst>
 </file>
@@ -190,10 +253,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -474,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,9 +554,9 @@
     <col min="1" max="1" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -561,39 +630,108 @@
       <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:25" s="4" customFormat="1" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
       <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
         <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
@@ -605,7 +743,7 @@
         <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
         <v>30</v>
@@ -614,99 +752,114 @@
         <v>31</v>
       </c>
       <c r="O3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="P3" t="s">
         <v>28</v>
       </c>
       <c r="Q3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="R3" t="s">
         <v>28</v>
       </c>
       <c r="S3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="T3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="U3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="V3" t="s">
         <v>28</v>
       </c>
       <c r="W3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="Y3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
       </c>
       <c r="P4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small bugfixes and improvements
</commit_message>
<xml_diff>
--- a/xTable_definition.xlsx
+++ b/xTable_definition.xlsx
@@ -110,9 +110,6 @@
     <t>str</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>list of floats</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>Position of the cross-linker within peptide2</t>
+  </si>
+  <si>
+    <t>pd.Int64Dtype()</t>
   </si>
 </sst>
 </file>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,76 +636,76 @@
         <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="W2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -716,70 +716,70 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
       </c>
       <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>30</v>
       </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
       <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
         <v>29</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
       </c>
       <c r="O3" t="s">
         <v>27</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="Q3" t="s">
         <v>27</v>
       </c>
       <c r="R3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="S3" t="s">
         <v>27</v>
       </c>
       <c r="T3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U3" t="s">
         <v>27</v>
       </c>
       <c r="V3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="W3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="X3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y3" t="s">
         <v>27</v>
@@ -787,79 +787,79 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplified XiFDR parser by using the _PSM_xiFDR file as sole data source
</commit_message>
<xml_diff>
--- a/xTable_definition.xlsx
+++ b/xTable_definition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>rawfile</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>pd.Int64Dtype()</t>
+  </si>
+  <si>
+    <t>mass of a modification within peptide2 (;-delimited if multiple)</t>
+  </si>
+  <si>
+    <t>mass of a modification within peptide1 (;-delimited if multiple)</t>
   </si>
 </sst>
 </file>
@@ -545,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +663,7 @@
         <v>56</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>55</v>
@@ -666,7 +672,7 @@
         <v>54</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>53</v>

</xml_diff>